<commit_message>
Clear original graph & create nodes
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -44,61 +44,61 @@
     <t xml:space="preserve">WAREHOUSE</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Tampines, lat: 23.23452, lon: 87.24553 </t>
+    <t xml:space="preserve">locationName:”Tampines”, lat: 23.23452, lon: 87.24553 </t>
   </si>
   <si>
     <t xml:space="preserve">Pickupp.io</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Pickupp HQ, lat: 23.23452, lon: 87.24553 </t>
+    <t xml:space="preserve">locationName:”Pickupp HQ”, lat: 23.23452, lon: 87.24553 </t>
   </si>
   <si>
     <t xml:space="preserve">Janio FTZ</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:FTZ SG, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”FTZ SG”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">Satsaco Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Satsaco HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”Satsaco HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">Greenlane Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Greenland HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”Greenland HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">Kerry Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Kerry HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”Kerry HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">Entrego Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Entrego HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”Entrego HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">2Go Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:2Go HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”2Go HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">Seko Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:Seko HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”Seko HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">GoJek Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">locationName:GoJek HQ, lat: 23.23452, lon: 87.24553</t>
+    <t xml:space="preserve">locationName:”GoJek HQ”, lat: 23.23452, lon: 87.24553</t>
   </si>
   <si>
     <t xml:space="preserve">Manila</t>
@@ -238,7 +238,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Edit logic to create the graph
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -125,16 +125,49 @@
     <t xml:space="preserve">node2_label</t>
   </si>
   <si>
-    <t xml:space="preserve">sf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPERATED_ON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cutoff:12, capacity:60, cost:78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">warehouse</t>
+    <t xml:space="preserve">CONNECTED_TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Pickupp.io', paymentType: 'COD', startTime: [7, 10, 13, 16], endTime: [9, 12, 15, 18], coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Pickupp.io', paymentType: 'NON_COD', startTime: [10, 13, 16, 18], endTime: [11, 14, 17, 20], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Janio Firstmile', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 40, via: 'Kerry', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Kerry', paymentType: 'NON_COD', startTime: 9, endTime: 11, handleableCapacity: 1200, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 18, via: 'Kerry', paymentType: 'NON_COD', startTime: [7, 10, 13, 16], endTime: [9, 12, 15, 18], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1500, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 22, via: 'Entrego', paymentType: 'COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 18, via: '2Go', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 22, via: 'Seko', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['ZI', 'UA']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 19, via: 'GoJek', paymentType: 'COD', startTime: [9, 12, 15, 18], endTime: [12, 15, 18, 21], handleableCapacity: 1000, restrictedMerchants: ['AA', 'UA']</t>
   </si>
 </sst>
 </file>
@@ -144,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -165,6 +198,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,13 +249,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -238,7 +282,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -405,17 +449,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="69.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
@@ -430,7 +475,7 @@
       <c r="C1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -440,18 +485,324 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run algo logic for single order and update order count
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" state="visible" r:id="rId2"/>
@@ -281,7 +281,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -451,8 +451,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,7 +485,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -505,7 +505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
@@ -525,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -545,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
@@ -565,7 +565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
@@ -605,7 +605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>12</v>
       </c>
@@ -625,7 +625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
@@ -645,7 +645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
@@ -665,7 +665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>16</v>
       </c>
@@ -685,7 +685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>16</v>
       </c>
@@ -705,7 +705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>16</v>
       </c>
@@ -725,7 +725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>18</v>
       </c>
@@ -745,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>20</v>
       </c>
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
@@ -785,7 +785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Return the path costs & links
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="53">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">Hougang</t>
   </si>
   <si>
-    <t xml:space="preserve">CITY</t>
+    <t xml:space="preserve">COVERAGEAREA</t>
   </si>
   <si>
     <t xml:space="preserve">Janio T-Space</t>
@@ -128,46 +128,58 @@
     <t xml:space="preserve">CONNECTED_TO</t>
   </si>
   <si>
-    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 25, via: 'Pickupp.io', paymentType: 'COD', startTime: [7, 10, 13, 16], endTime: [9, 12, 15, 18], coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 20, via: 'Pickupp.io', paymentType: 'NON_COD', startTime: [10, 13, 16, 18], endTime: [11, 14, 17, 20], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 25, via: 'Janio Firstmile', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 40, via: 'Kerry', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 25, via: 'Kerry', paymentType: 'NON_COD', startTime: 9, endTime: 11, handleableCapacity: 1200, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 18, via: 'Kerry', paymentType: 'NON_COD', startTime: [7, 10, 13, 16], endTime: [9, 12, 15, 18], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1500, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 22, via: 'Entrego', paymentType: 'COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 18, via: '2Go', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 22, via: 'Seko', paymentType: 'NON_COD', startTime: [8, 11, 14, 17], endTime: [10, 13, 16, 19], handleableCapacity: 1000, restrictedMerchants: ['ZI', 'UA']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost: 19, via: 'GoJek', paymentType: 'COD', startTime: [9, 12, 15, 18], endTime: [12, 15, 18, 21], handleableCapacity: 1000, restrictedMerchants: ['AA', 'UA']</t>
+    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'prepaid', startDate: datetime('2019-08-23T08:00:00’), endDate: datetime(‘2019-08-23T10:00:00’), coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'prepaid', startDate: datetime('2019-08-23T12:00:00’), endDate: datetime(‘2019-08-23T14:00:00’), coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Pickupp.io', paymentType: 'cod', startDate: datetime('2019-08-23T08:00:00’), endDate: datetime(‘2019-08-23T10:00:00’), coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Pickupp.io', paymentType: 'cod’, startDate: datetime('2019-08-23T12:00:00’), endDate: datetime(‘2019-08-23T17:00:00’), coverageArea: ['East', 'West'], handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Pickupp.io', paymentType: 'prepaid', startDate: datetime('2019-08-23T13:00:00’), endDate: datetime('2019-08-23T14:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'prepaid', startDate: datetime('2019-08-23T12:00:00’), endDate: datetime('2019-08-23T16:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Janio Firstmile', paymentType: 'prepaid', startDate: datetime('2019-08-24T10:00:00’), endDate: datetime('2019-08-24T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Janio Firstmile', paymentType: 'prepaid', startDate: datetime('2019-08-24T10:00:00’), endDate: datetime('2019-08-24T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'prepaid', startDate: datetime('2019-08-25T10:00:00’), endDate: datetime('2019-08-25T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 40, via: 'Kerry', paymentType: 'prepaid', startDate: datetime('2019-08-25T10:00:00’), endDate: datetime('2019-08-25T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'prepaid', startDate: datetime('2019-08-26T12:00:00’), endDate: datetime('2019-08-26T15:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 25, via: 'Kerry', paymentType: 'prepaid', startDate: datetime('2019-08-26T10:00:00’), endDate: datetime('2019-08-26T10:00:00’), handleableCapacity: 1200, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 18, via: 'Kerry', paymentType: 'prepaid', startDate: datetime('2019-08-26T10:00:00’), endDate: datetime('2019-08-26T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 20, via: 'Kerry', paymentType: 'prepaid', startDate: datetime('2019-08-23T10:00:00’), endDate: datetime('2019-08-23T10:00:00’), handleableCapacity: 1500, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 22, via: 'Entrego', paymentType: 'cod', startDate: datetime('2019-08-23T10:00:00’), endDate: datetime('2019-08-23T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 18, via: '2Go', paymentType: 'prepaid', startDate: datetime('2019-08-28T10:00:00’), endDate: datetime('2019-08-28T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'BB']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 22, via: 'Seko', paymentType: 'prepaid', startDate: datetime('2019-08-28T10:00:00’), endDate: datetime('2019-08-28T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['ZI', 'UA']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost: 19, via: 'GoJek', paymentType: 'cod', startDate: datetime('2019-08-23T10:00:00’), endDate: datetime('2019-08-23T10:00:00’), handleableCapacity: 1000, restrictedMerchants: ['AA', 'UA']</t>
   </si>
 </sst>
 </file>
@@ -282,7 +294,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -449,10 +461,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -462,7 +474,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="69.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
@@ -519,18 +532,18 @@
         <v>36</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>34</v>
@@ -539,18 +552,18 @@
         <v>37</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>34</v>
@@ -559,133 +572,133 @@
         <v>38</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="F6" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="F7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="F8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="F9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="F10" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="B11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="F11" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>16</v>
       </c>
@@ -696,16 +709,16 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>16</v>
       </c>
@@ -716,59 +729,59 @@
         <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="B16" s="0" t="s">
         <v>6</v>
       </c>
@@ -776,7 +789,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>26</v>
@@ -785,9 +798,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>6</v>
@@ -796,12 +809,52 @@
         <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>